<commit_message>
added the used C code for future purpose.
</commit_message>
<xml_diff>
--- a/c780_carel_cloud_engine_binary_Step_2/GME_stack_heap_analysis.xlsx
+++ b/c780_carel_cloud_engine_binary_Step_2/GME_stack_heap_analysis.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stack per Task" sheetId="1" r:id="rId1"/>
     <sheet name="Heap memory" sheetId="2" r:id="rId2"/>
-    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
+    <sheet name="Codice utilizzato" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -324,14 +324,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -566,11 +566,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="it-IT" sz="1100" b="1"/>
-            <a:t> di FreeRtos </a:t>
+            <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="it-IT" sz="1100" b="0"/>
-            <a:t>(this function </a:t>
+            <a:t>di FreeRtos (this function </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="it-IT" sz="1100" b="0" i="0">
@@ -1138,7 +1138,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="it-IT" sz="1100" baseline="0"/>
-            <a:t> rtcc...)</a:t>
+            <a:t> httpd,etc...)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1229,6 +1229,617 @@
             <a:rPr lang="it-IT" sz="1600"/>
             <a:t>112648</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CasellaDiTesto 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="228600"/>
+          <a:ext cx="8724900" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>I valori della heap memory sono statu ottenuti usando la funzione  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>esp_get_free_heap_size() </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>di FreeRtos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CasellaDiTesto 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="335280"/>
+          <a:ext cx="8724900" cy="4930140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NB: Per poter utilizzare le funzioni offerte da FreeRtos bisogna abilitarle via menuconfig entrando in:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       Component Config ----&gt; FreeRtos ----&gt;  [*] Enable freeRtos trace facility</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		                   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[*] Enable freeRtos stats formatting function</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NB: Il codice utilizza</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> un buffer da 800 bytes in relazione al fatto che</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         la funzione </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>vTaskList</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> necessità di 40bytes per task per immagazzinare i dati utili.</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>#include "freertos/task.h"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0" smtClean="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>char ptrTaskList[800];</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>void TaskInfo(void)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>printf("----------- heap:%u --------------\r\n", esp_get_free_heap_size());</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    vTaskList(ptrTaskList);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    printf("**********************************\r\n");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    printf("Task           State   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" u="none" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Prio    Stack    Num\r\n");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    printf("**********************************\r\n");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    printf(ptrTaskList);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    printf("\r\n**********************************\r\n");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100" b="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1526,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1669,7 +2280,7 @@
         <v>4096</v>
       </c>
       <c r="J18" s="12">
-        <f>G18 -E18</f>
+        <f t="shared" ref="J18:J23" si="0">G18 -E18</f>
         <v>768</v>
       </c>
     </row>
@@ -1696,7 +2307,7 @@
         <v>8192</v>
       </c>
       <c r="J19" s="12">
-        <f>G19 -E19</f>
+        <f t="shared" si="0"/>
         <v>3012</v>
       </c>
     </row>
@@ -1723,7 +2334,7 @@
         <v>1024</v>
       </c>
       <c r="J20" s="12">
-        <f>G20 -E20</f>
+        <f t="shared" si="0"/>
         <v>496</v>
       </c>
     </row>
@@ -1750,7 +2361,7 @@
         <v>7680</v>
       </c>
       <c r="J21" s="5">
-        <f>G21 -E21</f>
+        <f t="shared" si="0"/>
         <v>1700</v>
       </c>
     </row>
@@ -1777,7 +2388,7 @@
         <v>3072</v>
       </c>
       <c r="J22" s="5">
-        <f>G22 -E22</f>
+        <f t="shared" si="0"/>
         <v>1004</v>
       </c>
     </row>
@@ -1804,7 +2415,7 @@
         <v>2048</v>
       </c>
       <c r="J23" s="5">
-        <f>G23 -E23</f>
+        <f t="shared" si="0"/>
         <v>588</v>
       </c>
     </row>
@@ -1990,7 +2601,7 @@
         <v>1024</v>
       </c>
       <c r="J30" s="12">
-        <f t="shared" ref="J30:J31" si="0">G30 -E30</f>
+        <f t="shared" ref="J30:J31" si="1">G30 -E30</f>
         <v>476</v>
       </c>
     </row>
@@ -2017,7 +2628,7 @@
         <v>1024</v>
       </c>
       <c r="J31" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>476</v>
       </c>
     </row>
@@ -2168,7 +2779,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:A35">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="aggiunto">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="aggiunto">
       <formula>NOT(ISERROR(SEARCH("aggiunto",A34)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2217,7 +2828,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2231,10 +2842,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>